<commit_message>
06/11/2025 Ya funciona la exportción del comentario, no exporta no solventado, queda arreglar templates solventación para que vea una previsualización de lo ya solventado
</commit_message>
<xml_diff>
--- a/static/Plantilla.xlsx
+++ b/static/Plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Programas\SCIL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D294F91B-8B2C-4C2A-8654-4C20AF63DA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990448AD-0E0F-49A6-B2BC-EB9464A827C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>QNA12</t>
   </si>
   <si>
-    <t>TOT_NETO</t>
-  </si>
-  <si>
     <t>QNA13</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>QNA24</t>
+  </si>
+  <si>
+    <t>TOT_PERC</t>
   </si>
 </sst>
 </file>
@@ -524,11 +524,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="30" max="30" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -583,43 +586,43 @@
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>